<commit_message>
Add option to generate shop with multiple regions. Fix bug where the first region wasn't being loaded.
Signed-off-by: Nicolas <th3davinci00@mail.com>
</commit_message>
<xml_diff>
--- a/DynamicMarket.xlsx
+++ b/DynamicMarket.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="48" documentId="11_BB63D2749F0E83CBACEEA6C4CF4AAD3B15ED38A1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6633767D-91E9-48C2-AE69-B31C8FC6C2EB}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shops" sheetId="1" r:id="rId1"/>
@@ -916,8 +916,8 @@
   </sheetPr>
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1208,7 +1208,7 @@
   </sheetPr>
   <dimension ref="A1:Z980"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>

</xml_diff>